<commit_message>
Add separability results in csv
</commit_message>
<xml_diff>
--- a/ComputedResults/Area/SixBorderVowels/Danish/Formant/6_bordervowels_formant_da_ADS.xlsx
+++ b/ComputedResults/Area/SixBorderVowels/Danish/Formant/6_bordervowels_formant_da_ADS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,474 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AF</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>220504</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>140335</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>16</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>182923</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>145498</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>298328</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>JA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>24</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>388198</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>JE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>21</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>126746</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>KA</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>266515</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>KV</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>16</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>127320</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LK</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>16</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>259046</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LM</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>160641</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>16</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>199391</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>23</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>351306</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>175776</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MPS</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>183838</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>188156</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MV</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>178296</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>11</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>259467</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RV</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>209646</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>15</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>199035</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SAF</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>254853</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>19</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>198182</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>14</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>7336</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SS</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>14</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>170955</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TL</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>11</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>271789</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>TM</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ADS</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>246156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>